<commit_message>
Added first compare results for decode-sequencenumber-large
Change the CustomTraceAnalyzer to ouput a CSV for comparing the large
sequencenumber directory.
Added an excelsheet with the results. 4 sequencenumbers found!
</commit_message>
<xml_diff>
--- a/Logical-Analyzer-Captures/decode-sequencenumber/decode-sequencenumber.xlsx
+++ b/Logical-Analyzer-Captures/decode-sequencenumber/decode-sequencenumber.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="part1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -126,9 +126,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +166,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -238,7 +238,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2576,46 +2576,46 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>149</v>
       </c>
-      <c r="B26">
-        <v>89</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="1">
+        <v>89</v>
+      </c>
+      <c r="C26" s="1">
         <v>153</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>153</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>86</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>86</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>86</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>86</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>86</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <v>86</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="1">
         <v>86</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>86</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1">
         <v>86</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <v>86</v>
       </c>
     </row>

</xml_diff>